<commit_message>
se realiza cambio en promtp y archivo de texto
</commit_message>
<xml_diff>
--- a/numero_cliente.xlsx
+++ b/numero_cliente.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thder\OneDrive\Escritorio\trabajo\Chatbot_version_tesis\Nueva carpeta\chatbot\demo1_llamaIndex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D727F-A004-4E8F-B6AB-AA1D1F84F939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D997DCD-42BB-4998-AEDD-53AFFED247CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>cliente</t>
   </si>
@@ -428,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9729FC-45F9-4E8E-876D-940A8BDE57B2}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -488,6 +488,15 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>573185344536</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
cambios para que no responda preguntas no consultas
</commit_message>
<xml_diff>
--- a/numero_cliente.xlsx
+++ b/numero_cliente.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thder\OneDrive\Escritorio\trabajo\Chatbot_version_tesis\Nueva carpeta\chatbot\demo1_llamaIndex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D997DCD-42BB-4998-AEDD-53AFFED247CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12798308-14AD-490A-ADB2-D7F589C66ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="bd_clientes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>cliente</t>
   </si>
@@ -48,6 +49,30 @@
   </si>
   <si>
     <t>numero</t>
+  </si>
+  <si>
+    <t>Bases de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PST </t>
+  </si>
+  <si>
+    <t>CINTR</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>DEI</t>
+  </si>
+  <si>
+    <t>DBSGICOL</t>
+  </si>
+  <si>
+    <t>DBSGIECU</t>
+  </si>
+  <si>
+    <t>DBSGIPE</t>
   </si>
 </sst>
 </file>
@@ -430,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9729FC-45F9-4E8E-876D-940A8BDE57B2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,4 +526,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7CC7F1-F0A7-4852-8E4D-7A289156329C}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
detecta campos opcionales y el cliente por numero
</commit_message>
<xml_diff>
--- a/numero_cliente.xlsx
+++ b/numero_cliente.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thder\OneDrive\Escritorio\trabajo\Chatbot_version_tesis\Nueva carpeta\chatbot\demo1_llamaIndex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12798308-14AD-490A-ADB2-D7F589C66ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95F1B8F-7687-45B4-BC3D-11F9F3A35BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>cliente</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>DBSGIPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"http://192.168.169.23:8083/dbaexperts/dataBase" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"http://192.168.169.23:8083/dbaexperts/pst_dataBase" </t>
+  </si>
+  <si>
+    <t>links</t>
   </si>
 </sst>
 </file>
@@ -455,13 +464,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9729FC-45F9-4E8E-876D-940A8BDE57B2}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,69 +539,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7CC7F1-F0A7-4852-8E4D-7A289156329C}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios a documentos de carpeta data
</commit_message>
<xml_diff>
--- a/numero_cliente.xlsx
+++ b/numero_cliente.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thder\OneDrive\Escritorio\trabajo\Chatbot_version_tesis\Nueva carpeta\chatbot\demo1_llamaIndex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95F1B8F-7687-45B4-BC3D-11F9F3A35BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45617DFE-6D0F-4A15-96FC-60CE9509CB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AB433C97-C1FA-4758-832A-35EF26E79635}"/>
   </bookViews>
@@ -125,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +466,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +528,9 @@
         <v>573185344536</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>